<commit_message>
Updated naming convection for reference papers
</commit_message>
<xml_diff>
--- a/Requirements_Tech_Applications.xlsx
+++ b/Requirements_Tech_Applications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s555173_nwmissouri_edu/Documents/Desktop/GenerativeAI/GenerativeAI_ResearchPaper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="14_{5A3A477A-E747-4E20-A186-8DA868FC1270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F08E37D9-0C8F-43E0-B5BE-2A5C89041987}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="14_{5A3A477A-E747-4E20-A186-8DA868FC1270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1AFCC06-E8D0-4F53-B450-56912D2D89B2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{19148B62-65ED-4FF3-AA91-7AE7EF6C795A}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="283">
   <si>
     <t>Sl.No</t>
   </si>
@@ -513,9 +513,6 @@
     <t>Big GAN</t>
   </si>
   <si>
-    <t>KCYYXF_2017</t>
-  </si>
-  <si>
     <t>PYYKYZ_2019</t>
   </si>
   <si>
@@ -937,9 +934,6 @@
     <t>DCGAN (Deep Convolutional Generative Adversarial Network) with CNN</t>
   </si>
   <si>
-    <t>HGMMS_2020</t>
-  </si>
-  <si>
     <t>FWYFJ_2019</t>
   </si>
   <si>
@@ -988,9 +982,6 @@
     <t>Crystal Diffusion Variational autoencoders</t>
   </si>
   <si>
-    <t>ZMQMKTJ_2023</t>
-  </si>
-  <si>
     <t>ZJCGHSZ_2020</t>
   </si>
   <si>
@@ -1015,9 +1006,6 @@
     <t>T5 tranformer model with Tfix</t>
   </si>
   <si>
-    <t>ZCZCLCQYZ_2023</t>
-  </si>
-  <si>
     <t>BBHJRVVM_2021</t>
   </si>
   <si>
@@ -1042,49 +1030,87 @@
     <t>WT5(Why, T5?)</t>
   </si>
   <si>
-    <t>NSRCLKRAFNMK_2020</t>
-  </si>
-  <si>
     <t>translation,questionanswering,andclassification</t>
   </si>
   <si>
     <t>T5</t>
   </si>
   <si>
-    <t>RCSNRALKN_2020</t>
-  </si>
-  <si>
     <t>Generating images for captions</t>
   </si>
   <si>
     <t>alignDRAW (Deep Recurrent Attention Writer)</t>
   </si>
   <si>
-    <t>MEPEBJAR_2015</t>
-  </si>
-  <si>
     <t>DCGAN</t>
   </si>
   <si>
-    <t>RSAZYXLLSBLH_2016</t>
-  </si>
-  <si>
     <t>Generating more complex images for captions</t>
   </si>
   <si>
     <t>GALIP</t>
   </si>
   <si>
-    <t>TMBBTHXC_2023</t>
-  </si>
-  <si>
     <t>Generating speech from text</t>
   </si>
   <si>
     <t>FastSpeech</t>
   </si>
   <si>
-    <t>RYRYTXQTZSZZLT_2019</t>
+    <t>Video+Text</t>
+  </si>
+  <si>
+    <t>Editing Video based on text input &amp; 
+Image animation based on input (image+text)</t>
+  </si>
+  <si>
+    <t>Dreamix(Video Diffusion Models)</t>
+  </si>
+  <si>
+    <t>MHVA_2023</t>
+  </si>
+  <si>
+    <t>TBTX_2023</t>
+  </si>
+  <si>
+    <t>RAYL_2016</t>
+  </si>
+  <si>
+    <t>RRTQ_2019</t>
+  </si>
+  <si>
+    <t>MPBS_2015</t>
+  </si>
+  <si>
+    <t>RSRL_2020</t>
+  </si>
+  <si>
+    <t>NRLR_2020</t>
+  </si>
+  <si>
+    <t>WGDL_2017</t>
+  </si>
+  <si>
+    <t>BO_2023</t>
+  </si>
+  <si>
+    <t>The research paper contains inaccuracies in its references, 
+which are not aligned with the intended objectives of the study.</t>
+  </si>
+  <si>
+    <t>HGPR_2020</t>
+  </si>
+  <si>
+    <t>Education, Bussiness, Society</t>
+  </si>
+  <si>
+    <t>DKHS_2023</t>
+  </si>
+  <si>
+    <t>ZZLQ_2023</t>
+  </si>
+  <si>
+    <t>ZQKJ_2023</t>
   </si>
 </sst>
 </file>
@@ -1689,10 +1715,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24709A7D-2AAA-43FD-A6AD-A1AB49C8346D}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1800,6 +1826,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>280</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D8" s="10">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1807,10 +1847,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A003E202-2296-40B6-97C5-6ED01973FD6A}">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="76" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="76" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1821,7 +1861,7 @@
     <col min="4" max="4" width="63.54296875" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.7265625" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="139.36328125" style="10" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12.08984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6328125" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.81640625" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.7265625" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.81640625" style="10" bestFit="1" customWidth="1"/>
@@ -1854,7 +1894,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>37</v>
@@ -1874,7 +1914,7 @@
         <v>65</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>43</v>
@@ -1886,7 +1926,7 @@
         <v>2</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>45</v>
@@ -1918,7 +1958,7 @@
         <v>9</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>45</v>
@@ -1938,7 +1978,7 @@
         <v>61</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>47</v>
@@ -1950,7 +1990,7 @@
         <v>16</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>45</v>
@@ -1970,7 +2010,7 @@
         <v>49</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>89</v>
@@ -1982,7 +2022,7 @@
         <v>17</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>45</v>
@@ -2002,7 +2042,7 @@
         <v>91</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>90</v>
@@ -2014,7 +2054,7 @@
         <v>17</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J6" s="11"/>
     </row>
@@ -2032,7 +2072,7 @@
         <v>62</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>63</v>
@@ -2044,7 +2084,7 @@
         <v>19</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>45</v>
@@ -2064,7 +2104,7 @@
         <v>64</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>53</v>
@@ -2076,7 +2116,7 @@
         <v>19</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>45</v>
@@ -2096,7 +2136,7 @@
         <v>51</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11" t="s">
@@ -2106,7 +2146,7 @@
         <v>20</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>45</v>
@@ -2126,7 +2166,7 @@
         <v>55</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
@@ -2134,7 +2174,7 @@
         <v>21</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>45</v>
@@ -2166,7 +2206,7 @@
         <v>13</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>45</v>
@@ -2183,10 +2223,10 @@
         <v>74</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8" t="s">
@@ -2196,7 +2236,7 @@
         <v>12</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>45</v>
@@ -2216,7 +2256,7 @@
         <v>66</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>67</v>
@@ -2228,13 +2268,13 @@
         <v>19</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -2260,7 +2300,7 @@
         <v>20</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>45</v>
@@ -2280,7 +2320,7 @@
         <v>71</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>72</v>
@@ -2292,7 +2332,7 @@
         <v>85</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>45</v>
@@ -2312,7 +2352,7 @@
         <v>73</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11" t="s">
@@ -2322,7 +2362,7 @@
         <v>25</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>45</v>
@@ -2342,7 +2382,7 @@
         <v>75</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>76</v>
@@ -2354,7 +2394,7 @@
         <v>28</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J17" s="11" t="s">
         <v>45</v>
@@ -2386,7 +2426,7 @@
         <v>28</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>45</v>
@@ -2418,7 +2458,7 @@
         <v>28</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>45</v>
@@ -2441,16 +2481,16 @@
         <v>101</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>113</v>
+        <v>275</v>
       </c>
       <c r="H20" s="10">
         <v>6</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2470,16 +2510,16 @@
         <v>102</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>113</v>
+        <v>275</v>
       </c>
       <c r="H21" s="10">
         <v>6</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2499,16 +2539,16 @@
         <v>103</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>113</v>
+        <v>275</v>
       </c>
       <c r="H22" s="10">
         <v>6</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
@@ -2528,16 +2568,16 @@
         <v>104</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>113</v>
+        <v>275</v>
       </c>
       <c r="H23" s="10">
         <v>7</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -2557,16 +2597,16 @@
         <v>105</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H24" s="10">
         <v>7</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2586,16 +2626,16 @@
         <v>106</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H25" s="10">
         <v>7</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2615,16 +2655,16 @@
         <v>107</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H26" s="10">
         <v>7</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2644,16 +2684,16 @@
         <v>108</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H27" s="10">
         <v>7</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -2673,16 +2713,16 @@
         <v>109</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H28" s="10">
         <v>7</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -2702,16 +2742,16 @@
         <v>110</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H29" s="10">
         <v>7</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -2731,16 +2771,16 @@
         <v>111</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H30" s="10">
         <v>7</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2760,16 +2800,16 @@
         <v>112</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H31" s="10">
         <v>7</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2777,25 +2817,25 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>50</v>
       </c>
       <c r="D32" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="G32" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>153</v>
       </c>
       <c r="H32" s="10">
         <v>6</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J32" s="10" t="s">
         <v>45</v>
@@ -2806,25 +2846,25 @@
         <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C33" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="E33" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="E33" s="12" t="s">
-        <v>157</v>
-      </c>
       <c r="G33" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H33" s="10">
         <v>6</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J33" s="10" t="s">
         <v>45</v>
@@ -2838,22 +2878,22 @@
         <v>40</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D34" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" s="10" t="s">
         <v>162</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>163</v>
       </c>
       <c r="H34" s="10">
         <v>4</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J34" s="10" t="s">
         <v>45</v>
@@ -2870,19 +2910,19 @@
         <v>41</v>
       </c>
       <c r="D35" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E35" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="G35" s="10" t="s">
         <v>167</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>168</v>
       </c>
       <c r="H35" s="10">
         <v>6</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J35" s="10" t="s">
         <v>45</v>
@@ -2893,25 +2933,25 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C36" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="D36" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="E36" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="G36" s="10" t="s">
         <v>184</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>185</v>
       </c>
       <c r="H36" s="10">
         <v>4</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J36" s="10" t="s">
         <v>45</v>
@@ -2928,19 +2968,19 @@
         <v>40</v>
       </c>
       <c r="D37" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="G37" s="10" t="s">
         <v>191</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>192</v>
       </c>
       <c r="H37" s="10">
         <v>10</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2951,22 +2991,22 @@
         <v>41</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H38" s="10">
         <v>11</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
@@ -2980,19 +3020,19 @@
         <v>41</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H39" s="10">
         <v>12</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
@@ -3006,13 +3046,13 @@
         <v>41</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H40" s="10">
         <v>12</v>
@@ -3029,13 +3069,13 @@
         <v>41</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
@@ -3049,13 +3089,13 @@
         <v>41</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
@@ -3063,19 +3103,19 @@
         <v>42</v>
       </c>
       <c r="B43" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C43" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="D43" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="E43" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="D43" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>207</v>
-      </c>
       <c r="G43" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
@@ -3089,16 +3129,16 @@
         <v>41</v>
       </c>
       <c r="D44" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="E44" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="G44" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="I44" s="12" t="s">
         <v>213</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="I44" s="12" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
@@ -3109,16 +3149,16 @@
         <v>41</v>
       </c>
       <c r="C45" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D45" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="E45" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="E45" s="10" t="s">
-        <v>217</v>
-      </c>
       <c r="G45" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
@@ -3132,16 +3172,16 @@
         <v>41</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E46" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="I46" s="10" t="s">
         <v>219</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="I46" s="10" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
@@ -3149,28 +3189,28 @@
         <v>46</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D47" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="E47" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="E47" s="10" t="s">
-        <v>224</v>
-      </c>
       <c r="G47" s="10" t="s">
-        <v>225</v>
+        <v>278</v>
       </c>
       <c r="H47" s="10">
         <v>12</v>
       </c>
       <c r="I47" s="10" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
@@ -3178,28 +3218,28 @@
         <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="E48" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="C48" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>229</v>
-      </c>
       <c r="G48" s="10" t="s">
-        <v>225</v>
+        <v>278</v>
       </c>
       <c r="H48" s="10">
         <v>14</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
@@ -3207,28 +3247,28 @@
         <v>48</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>225</v>
+        <v>278</v>
       </c>
       <c r="H49" s="10">
         <v>9</v>
       </c>
       <c r="I49" s="10" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
@@ -3236,28 +3276,28 @@
         <v>49</v>
       </c>
       <c r="B50" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D50" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="E50" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="D50" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>237</v>
-      </c>
       <c r="G50" s="10" t="s">
-        <v>225</v>
+        <v>278</v>
       </c>
       <c r="H50" s="10">
         <v>10</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
@@ -3265,28 +3305,28 @@
         <v>50</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C51" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="E51" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="D51" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>241</v>
-      </c>
       <c r="G51" s="10" t="s">
-        <v>242</v>
+        <v>282</v>
       </c>
       <c r="H51" s="10">
         <v>8</v>
       </c>
       <c r="I51" s="10" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
@@ -3294,28 +3334,28 @@
         <v>51</v>
       </c>
       <c r="B52" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="E52" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C52" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>247</v>
-      </c>
       <c r="G52" s="10" t="s">
-        <v>242</v>
+        <v>282</v>
       </c>
       <c r="H52" s="10">
         <v>7</v>
       </c>
       <c r="I52" s="10" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
@@ -3329,22 +3369,22 @@
         <v>40</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>251</v>
+        <v>281</v>
       </c>
       <c r="H53" s="10">
         <v>20</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
@@ -3352,28 +3392,28 @@
         <v>53</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C54" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>251</v>
+        <v>281</v>
       </c>
       <c r="H54" s="10">
         <v>20</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
@@ -3381,28 +3421,28 @@
         <v>54</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>251</v>
+        <v>281</v>
       </c>
       <c r="H55" s="10">
         <v>20</v>
       </c>
       <c r="I55" s="10" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
@@ -3410,28 +3450,28 @@
         <v>55</v>
       </c>
       <c r="B56" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="E56" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="C56" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>262</v>
-      </c>
       <c r="G56" s="10" t="s">
-        <v>251</v>
+        <v>281</v>
       </c>
       <c r="H56" s="10">
         <v>20</v>
       </c>
       <c r="I56" s="10" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.35">
@@ -3439,28 +3479,28 @@
         <v>56</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>251</v>
+        <v>281</v>
       </c>
       <c r="H57" s="10">
         <v>20</v>
       </c>
       <c r="I57" s="10" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.35">
@@ -3468,28 +3508,28 @@
         <v>57</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>251</v>
+        <v>281</v>
       </c>
       <c r="H58" s="10">
         <v>20</v>
       </c>
       <c r="I58" s="10" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="J58" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.35">
@@ -3497,28 +3537,28 @@
         <v>58</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>251</v>
+        <v>281</v>
       </c>
       <c r="H59" s="10">
         <v>20</v>
       </c>
       <c r="I59" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J59" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.35">
@@ -3526,28 +3566,57 @@
         <v>59</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>251</v>
+        <v>281</v>
       </c>
       <c r="H60" s="10">
         <v>20</v>
       </c>
       <c r="I60" s="10" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A61" s="10">
+        <v>60</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="H61" s="10">
+        <v>20</v>
+      </c>
+      <c r="I61" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="J61" s="10" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -3559,10 +3628,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B24F9BD-DBB3-4699-BEB1-125B6EBE7265}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3572,28 +3641,36 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" t="s">
         <v>180</v>
-      </c>
-      <c r="B3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" t="s">
         <v>188</v>
-      </c>
-      <c r="B4" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>276</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Pratap Review Work
</commit_message>
<xml_diff>
--- a/Requirements_Tech_Applications.xlsx
+++ b/Requirements_Tech_Applications.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s555173_nwmissouri_edu/Documents/Desktop/GenerativeAI/GenerativeAI_ResearchPaper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s555080_nwmissouri_edu/Documents/Desktop/Generative AI/Git Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="14_{5A3A477A-E747-4E20-A186-8DA868FC1270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1AFCC06-E8D0-4F53-B450-56912D2D89B2}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="14_{5A3A477A-E747-4E20-A186-8DA868FC1270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E3488E3-00BA-4A91-A0CF-A6567A5A873F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{19148B62-65ED-4FF3-AA91-7AE7EF6C795A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" activeTab="3" xr2:uid="{19148B62-65ED-4FF3-AA91-7AE7EF6C795A}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Applications" sheetId="3" r:id="rId3"/>
     <sheet name="Taxonomy" sheetId="4" r:id="rId4"/>
     <sheet name="Excluded" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Taxonomy!$A$1:$J$43</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="266">
   <si>
     <t>Sl.No</t>
   </si>
@@ -513,6 +514,9 @@
     <t>Big GAN</t>
   </si>
   <si>
+    <t>KCYYXF_2017</t>
+  </si>
+  <si>
     <t>PYYKYZ_2019</t>
   </si>
   <si>
@@ -866,9 +870,6 @@
     <t>Ex-GAN,CA-GAN, PG-GAN</t>
   </si>
   <si>
-    <t>Age-CGAN, CAAE, IP-CGAN, PG-GAN</t>
-  </si>
-  <si>
     <t>AttnGAN, StackGAN, ACGAN, TACGAN, SISGAN</t>
   </si>
   <si>
@@ -878,239 +879,186 @@
     <t>Stego Image/Image</t>
   </si>
   <si>
-    <t>SGAN</t>
-  </si>
-  <si>
     <t>DR-GAN, PG-GAN, PS-CGAN</t>
   </si>
   <si>
-    <t>KAHK_2017,KALL_2018,
+    <t>WZZH_2019,CK_2019</t>
+  </si>
+  <si>
+    <t>Hiding Secret Message in an Image/Steganography</t>
+  </si>
+  <si>
+    <t>convert our rough sketch to realstic image</t>
+  </si>
+  <si>
+    <t>IGAN,TA-GAN,IAN,Att-GAN,D-GAN</t>
+  </si>
+  <si>
+    <t>Image/Segmentation Mask</t>
+  </si>
+  <si>
+    <t>Medical Image Analysis/Segment the Objects Or Regions in an Image</t>
+  </si>
+  <si>
+    <t>SegAN</t>
+  </si>
+  <si>
+    <t>JLRN_2021</t>
+  </si>
+  <si>
+    <t>Staingan,PathologyGAN</t>
+  </si>
+  <si>
+    <t>SBNA_2018,QSY_2021</t>
+  </si>
+  <si>
+    <t>Helps in classification of Tumors etc in an image/Helps in Pathology Domain</t>
+  </si>
+  <si>
+    <t>To Generate High Quality Images</t>
+  </si>
+  <si>
+    <t>LAPGAN</t>
+  </si>
+  <si>
+    <t>DCSF_2015</t>
+  </si>
+  <si>
+    <t>CJCL_2018</t>
+  </si>
+  <si>
+    <t>Converting a Low Resolution Image to High Resolution Image</t>
+  </si>
+  <si>
+    <t>SRGAN</t>
+  </si>
+  <si>
+    <t>CT_2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To generate realstic images </t>
+  </si>
+  <si>
+    <t>SAGAN</t>
+  </si>
+  <si>
+    <t>ZGMO_2019</t>
+  </si>
+  <si>
+    <t>Style Transfer(Black &amp; White Image to Color Image)</t>
+  </si>
+  <si>
+    <t>Pix2Pix</t>
+  </si>
+  <si>
+    <t>IZZE_2019</t>
+  </si>
+  <si>
+    <t>Style Transfer(Cartoon to Image or Painting to Photgraph Or Apple to Orange)</t>
+  </si>
+  <si>
+    <t>KCKK_2017</t>
+  </si>
+  <si>
+    <t>Style Transfer</t>
+  </si>
+  <si>
+    <t>Cartoon Image to Real Image/Photo</t>
+  </si>
+  <si>
+    <t>DTN</t>
+  </si>
+  <si>
+    <t>TPW_2016</t>
+  </si>
+  <si>
+    <t>ZXLZ_2017</t>
+  </si>
+  <si>
+    <t>GAN-CLS</t>
+  </si>
+  <si>
+    <t>GX_2018</t>
+  </si>
+  <si>
+    <t>Various Frontal View Synthesis from Single face Image</t>
+  </si>
+  <si>
+    <t>TP-GAN</t>
+  </si>
+  <si>
+    <t>HZLH_2017</t>
+  </si>
+  <si>
+    <t>Image Restoration</t>
+  </si>
+  <si>
+    <t>PGGAN</t>
+  </si>
+  <si>
+    <t>KALL_2017</t>
+  </si>
+  <si>
+    <t>KAHK_2017,KALL_2017,
 HTLH_2018</t>
   </si>
   <si>
-    <t>WZZH_2019,CK_2019</t>
-  </si>
-  <si>
-    <t>Hiding Secret Message in an Image/Steganography</t>
-  </si>
-  <si>
-    <t>convert our rough sketch to realstic image</t>
-  </si>
-  <si>
-    <t>IGAN,TA-GAN,IAN,Att-GAN,D-GAN</t>
-  </si>
-  <si>
-    <t>ZKSE_2018,NKK_2018, 
-BLRW_2017, XZHZ_2017,BZSZ_2018</t>
-  </si>
-  <si>
-    <t>Image/Segmentation Mask</t>
-  </si>
-  <si>
-    <t>Medical Image Analysis/Segment the Objects Or Regions in an Image</t>
-  </si>
-  <si>
-    <t>SegAN</t>
-  </si>
-  <si>
-    <t>JLRN_2021</t>
-  </si>
-  <si>
-    <t>Staingan,PathologyGAN</t>
-  </si>
-  <si>
-    <t>SBNA_2018,QSY_2021</t>
-  </si>
-  <si>
-    <t>Helps in classification of Tumors etc in an image/Helps in Pathology Domain</t>
-  </si>
-  <si>
-    <t>Gesture</t>
-  </si>
-  <si>
-    <t>Gesture recognition</t>
-  </si>
-  <si>
-    <t>DCGAN (Deep Convolutional Generative Adversarial Network) with CNN</t>
-  </si>
-  <si>
-    <t>FWYFJ_2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speech </t>
-  </si>
-  <si>
-    <t>Speech enhancement</t>
-  </si>
-  <si>
-    <t>CGAN with pix to pix framework</t>
-  </si>
-  <si>
-    <t>MDTZ_2017</t>
-  </si>
-  <si>
-    <t>Spoken query detection</t>
-  </si>
-  <si>
-    <t>Deep Boltzmann Machines</t>
-  </si>
-  <si>
-    <t>ZYSRCH_2012</t>
-  </si>
-  <si>
-    <t>Graphs</t>
-  </si>
-  <si>
-    <t>Molecule Structure</t>
-  </si>
-  <si>
-    <t>Molecule generation</t>
-  </si>
-  <si>
-    <t>Variational autoencoders</t>
-  </si>
-  <si>
-    <t>LQAMBMGA_2018</t>
-  </si>
-  <si>
-    <t>Graph (Reconstructed)</t>
-  </si>
-  <si>
-    <t>Material Redesign</t>
-  </si>
-  <si>
-    <t>Crystal Diffusion Variational autoencoders</t>
-  </si>
-  <si>
-    <t>ZJCGHSZ_2020</t>
-  </si>
-  <si>
-    <t>2D Structure Molecule</t>
-  </si>
-  <si>
-    <t>3D Structure Molecule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generating 3D molecular structure </t>
-  </si>
-  <si>
-    <t>Geometry-complete diffusion model</t>
-  </si>
-  <si>
-    <t>MACJ_2023</t>
-  </si>
-  <si>
-    <t>Correcting Code errors</t>
-  </si>
-  <si>
-    <t>T5 tranformer model with Tfix</t>
-  </si>
-  <si>
-    <t>BBHJRVVM_2021</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Natural language generation from structured data</t>
-  </si>
-  <si>
-    <t>T5 tranformer model</t>
-  </si>
-  <si>
-    <t>KMRA_2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Text </t>
-  </si>
-  <si>
-    <t>Explaining the given statement</t>
-  </si>
-  <si>
-    <t>WT5(Why, T5?)</t>
-  </si>
-  <si>
-    <t>translation,questionanswering,andclassification</t>
-  </si>
-  <si>
-    <t>T5</t>
-  </si>
-  <si>
-    <t>Generating images for captions</t>
-  </si>
-  <si>
-    <t>alignDRAW (Deep Recurrent Attention Writer)</t>
-  </si>
-  <si>
-    <t>DCGAN</t>
-  </si>
-  <si>
-    <t>Generating more complex images for captions</t>
-  </si>
-  <si>
-    <t>GALIP</t>
-  </si>
-  <si>
-    <t>Generating speech from text</t>
-  </si>
-  <si>
-    <t>FastSpeech</t>
-  </si>
-  <si>
-    <t>Video+Text</t>
-  </si>
-  <si>
-    <t>Editing Video based on text input &amp; 
-Image animation based on input (image+text)</t>
-  </si>
-  <si>
-    <t>Dreamix(Video Diffusion Models)</t>
-  </si>
-  <si>
-    <t>MHVA_2023</t>
-  </si>
-  <si>
-    <t>TBTX_2023</t>
-  </si>
-  <si>
-    <t>RAYL_2016</t>
-  </si>
-  <si>
-    <t>RRTQ_2019</t>
-  </si>
-  <si>
-    <t>MPBS_2015</t>
-  </si>
-  <si>
-    <t>RSRL_2020</t>
-  </si>
-  <si>
-    <t>NRLR_2020</t>
-  </si>
-  <si>
-    <t>WGDL_2017</t>
-  </si>
-  <si>
-    <t>BO_2023</t>
-  </si>
-  <si>
-    <t>The research paper contains inaccuracies in its references, 
-which are not aligned with the intended objectives of the study.</t>
-  </si>
-  <si>
-    <t>HGPR_2020</t>
-  </si>
-  <si>
-    <t>Education, Bussiness, Society</t>
-  </si>
-  <si>
-    <t>DKHS_2023</t>
-  </si>
-  <si>
-    <t>ZZLQ_2023</t>
-  </si>
-  <si>
-    <t>ZQKJ_2023</t>
+    <t>DF_2018,YLYS_2018,DU_2018</t>
+  </si>
+  <si>
+    <t>Age-CGAN, CAAE, IP-CGAN</t>
+  </si>
+  <si>
+    <t>RQ1</t>
+  </si>
+  <si>
+    <t>Req</t>
+  </si>
+  <si>
+    <t>RQ2</t>
+  </si>
+  <si>
+    <t>tech</t>
+  </si>
+  <si>
+    <t>RQ3</t>
+  </si>
+  <si>
+    <t>Emerging Applications</t>
+  </si>
+  <si>
+    <t>Do IEEE&amp;ACM Same Research</t>
+  </si>
+  <si>
+    <t>ABD_2017,ZSQ_2017,WTS_2017</t>
+  </si>
+  <si>
+    <t>XZHZ_2017,ZXLZ_2017,OSS_2017,DGAL_2017,DYWG_2017</t>
+  </si>
+  <si>
+    <t>SGAN,SSGAN,Stegano-GAN</t>
+  </si>
+  <si>
+    <t>VNB_2019,SDWQ_2018,ZIXV_2019</t>
+  </si>
+  <si>
+    <t>ZKSE_2016,NKK_2018, 
+BLRW_2016, XZHZ_2017,BZSZ_2018</t>
+  </si>
+  <si>
+    <t>XXZL_2018</t>
+  </si>
+  <si>
+    <t>Future Market Prediction based on historical data</t>
+  </si>
+  <si>
+    <t>GAN-FD, ST-GAN,MTSGAN</t>
+  </si>
+  <si>
+    <t>ZPHT_2018,MZ_2021,WHKC_2021</t>
+  </si>
+  <si>
+    <t>EO_2021</t>
   </si>
 </sst>
 </file>
@@ -1522,7 +1470,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1715,10 +1663,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24709A7D-2AAA-43FD-A6AD-A1AB49C8346D}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1826,20 +1774,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>280</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="D8" s="10">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1847,10 +1781,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A003E202-2296-40B6-97C5-6ED01973FD6A}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="76" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="103" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1858,12 +1792,12 @@
     <col min="1" max="1" width="8.7265625" style="10"/>
     <col min="2" max="2" width="18.36328125" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.36328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.36328125" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.7265625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="139.36328125" style="10" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36" style="10" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.81640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.81640625" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="8.7265625" style="10"/>
   </cols>
@@ -1894,7 +1828,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>37</v>
@@ -1914,7 +1848,7 @@
         <v>65</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>43</v>
@@ -1926,7 +1860,7 @@
         <v>2</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>45</v>
@@ -1958,7 +1892,7 @@
         <v>9</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>45</v>
@@ -1978,7 +1912,7 @@
         <v>61</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>47</v>
@@ -1990,7 +1924,7 @@
         <v>16</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>45</v>
@@ -2010,7 +1944,7 @@
         <v>49</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>89</v>
@@ -2022,7 +1956,7 @@
         <v>17</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>45</v>
@@ -2042,7 +1976,7 @@
         <v>91</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>90</v>
@@ -2054,7 +1988,7 @@
         <v>17</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J6" s="11"/>
     </row>
@@ -2072,7 +2006,7 @@
         <v>62</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>63</v>
@@ -2084,7 +2018,7 @@
         <v>19</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>45</v>
@@ -2104,7 +2038,7 @@
         <v>64</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>53</v>
@@ -2116,7 +2050,7 @@
         <v>19</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>45</v>
@@ -2136,7 +2070,7 @@
         <v>51</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11" t="s">
@@ -2146,7 +2080,7 @@
         <v>20</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>45</v>
@@ -2166,7 +2100,7 @@
         <v>55</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
@@ -2174,7 +2108,7 @@
         <v>21</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>45</v>
@@ -2206,7 +2140,7 @@
         <v>13</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>45</v>
@@ -2223,10 +2157,10 @@
         <v>74</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8" t="s">
@@ -2236,7 +2170,7 @@
         <v>12</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>45</v>
@@ -2256,7 +2190,7 @@
         <v>66</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>67</v>
@@ -2268,13 +2202,13 @@
         <v>19</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -2300,7 +2234,7 @@
         <v>20</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>45</v>
@@ -2320,7 +2254,7 @@
         <v>71</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>72</v>
@@ -2332,7 +2266,7 @@
         <v>85</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>45</v>
@@ -2352,7 +2286,7 @@
         <v>73</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11" t="s">
@@ -2362,7 +2296,7 @@
         <v>25</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>45</v>
@@ -2382,7 +2316,7 @@
         <v>75</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>76</v>
@@ -2394,7 +2328,7 @@
         <v>28</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J17" s="11" t="s">
         <v>45</v>
@@ -2426,7 +2360,7 @@
         <v>28</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>45</v>
@@ -2458,7 +2392,7 @@
         <v>28</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>45</v>
@@ -2481,16 +2415,16 @@
         <v>101</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>275</v>
+        <v>113</v>
       </c>
       <c r="H20" s="10">
         <v>6</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2510,16 +2444,16 @@
         <v>102</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>275</v>
+        <v>113</v>
       </c>
       <c r="H21" s="10">
         <v>6</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2539,16 +2473,16 @@
         <v>103</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>275</v>
+        <v>113</v>
       </c>
       <c r="H22" s="10">
         <v>6</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
@@ -2568,16 +2502,16 @@
         <v>104</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>275</v>
+        <v>113</v>
       </c>
       <c r="H23" s="10">
         <v>7</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -2597,16 +2531,16 @@
         <v>105</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H24" s="10">
         <v>7</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2626,16 +2560,16 @@
         <v>106</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H25" s="10">
         <v>7</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2655,16 +2589,16 @@
         <v>107</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H26" s="10">
         <v>7</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2684,16 +2618,16 @@
         <v>108</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H27" s="10">
         <v>7</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -2713,16 +2647,16 @@
         <v>109</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H28" s="10">
         <v>7</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -2742,16 +2676,16 @@
         <v>110</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H29" s="10">
         <v>7</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -2771,16 +2705,16 @@
         <v>111</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H30" s="10">
         <v>7</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2800,16 +2734,16 @@
         <v>112</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H31" s="10">
         <v>7</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2817,25 +2751,25 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>50</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H32" s="10">
         <v>6</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J32" s="10" t="s">
         <v>45</v>
@@ -2846,25 +2780,25 @@
         <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H33" s="10">
         <v>6</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J33" s="10" t="s">
         <v>45</v>
@@ -2878,22 +2812,22 @@
         <v>40</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E34" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="G34" s="10" t="s">
         <v>163</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>162</v>
       </c>
       <c r="H34" s="10">
         <v>4</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="J34" s="10" t="s">
         <v>45</v>
@@ -2910,19 +2844,19 @@
         <v>41</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H35" s="10">
         <v>6</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J35" s="10" t="s">
         <v>45</v>
@@ -2933,25 +2867,25 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E36" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="G36" s="10" t="s">
         <v>185</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>184</v>
       </c>
       <c r="H36" s="10">
         <v>4</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J36" s="10" t="s">
         <v>45</v>
@@ -2968,19 +2902,19 @@
         <v>40</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E37" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="G37" s="10" t="s">
         <v>192</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>191</v>
       </c>
       <c r="H37" s="10">
         <v>10</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2991,22 +2925,22 @@
         <v>41</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H38" s="10">
         <v>11</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>208</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
@@ -3020,19 +2954,19 @@
         <v>41</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H39" s="10">
         <v>12</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
@@ -3046,16 +2980,19 @@
         <v>41</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H40" s="10">
         <v>12</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
@@ -3069,13 +3006,19 @@
         <v>41</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>202</v>
+        <v>248</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>191</v>
+        <v>192</v>
+      </c>
+      <c r="H41" s="10">
+        <v>12</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
@@ -3089,13 +3032,19 @@
         <v>41</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E42" s="10" t="s">
         <v>203</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>191</v>
+        <v>192</v>
+      </c>
+      <c r="H42" s="10">
+        <v>12</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
@@ -3109,16 +3058,22 @@
         <v>205</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>206</v>
+        <v>258</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+      <c r="H43" s="10">
+        <v>12</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="10">
         <v>43</v>
       </c>
@@ -3129,16 +3084,19 @@
         <v>41</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>191</v>
+        <v>192</v>
+      </c>
+      <c r="H44" s="10">
+        <v>12</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>213</v>
+        <v>260</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
@@ -3149,16 +3107,22 @@
         <v>41</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>191</v>
+        <v>192</v>
+      </c>
+      <c r="H45" s="10">
+        <v>12</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
@@ -3172,16 +3136,19 @@
         <v>41</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>217</v>
+        <v>214</v>
+      </c>
+      <c r="H46" s="10">
+        <v>4</v>
       </c>
       <c r="I46" s="10" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
@@ -3189,28 +3156,25 @@
         <v>46</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>221</v>
+        <v>41</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>278</v>
+        <v>214</v>
       </c>
       <c r="H47" s="10">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I47" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="J47" s="10" t="s">
-        <v>114</v>
+        <v>216</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
@@ -3218,405 +3182,282 @@
         <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>225</v>
+        <v>41</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>159</v>
+        <v>41</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>278</v>
+        <v>221</v>
       </c>
       <c r="H48" s="10">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="J48" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="10">
         <v>48</v>
       </c>
       <c r="B49" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D49" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="C49" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>229</v>
-      </c>
       <c r="E49" s="10" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>278</v>
+        <v>221</v>
       </c>
       <c r="H49" s="10">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I49" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="J49" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="10">
         <v>49</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>232</v>
+        <v>41</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>233</v>
+        <v>41</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>235</v>
+        <v>228</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>229</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>278</v>
+        <v>221</v>
       </c>
       <c r="H50" s="10">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="J50" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="10">
         <v>50</v>
       </c>
       <c r="B51" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="H51" s="10">
+        <v>13</v>
+      </c>
+      <c r="I51" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C51" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="G51" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="H51" s="10">
-        <v>8</v>
-      </c>
-      <c r="I51" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="J51" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="10">
         <v>51</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>241</v>
+        <v>41</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>242</v>
+        <v>41</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>244</v>
+        <v>107</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>282</v>
+        <v>221</v>
       </c>
       <c r="H52" s="10">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I52" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="J52" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="10">
         <v>52</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>281</v>
+        <v>221</v>
       </c>
       <c r="H53" s="10">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="J53" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="10">
         <v>53</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>249</v>
+        <v>40</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>250</v>
+        <v>41</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>251</v>
+        <v>104</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>281</v>
+        <v>221</v>
       </c>
       <c r="H54" s="10">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="J54" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="10">
         <v>54</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>253</v>
+        <v>40</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="D55" s="10" t="s">
-        <v>254</v>
+        <v>41</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>281</v>
+        <v>221</v>
       </c>
       <c r="H55" s="10">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I55" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="J55" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="10">
         <v>55</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>253</v>
+        <v>41</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>253</v>
+        <v>41</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>281</v>
+        <v>221</v>
       </c>
       <c r="H56" s="10">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I56" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="J56" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="10">
         <v>56</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>253</v>
+        <v>41</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>281</v>
+        <v>221</v>
       </c>
       <c r="H57" s="10">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I57" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="J57" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="10">
         <v>57</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>253</v>
+        <v>40</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="H58" s="10">
-        <v>20</v>
+        <v>265</v>
       </c>
       <c r="I58" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="J58" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A59" s="10">
-        <v>58</v>
-      </c>
-      <c r="B59" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D59" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="E59" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="G59" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="H59" s="10">
-        <v>20</v>
-      </c>
-      <c r="I59" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="J59" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A60" s="10">
-        <v>59</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="E60" s="10" t="s">
         <v>264</v>
-      </c>
-      <c r="G60" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="H60" s="10">
-        <v>20</v>
-      </c>
-      <c r="I60" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="J60" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A61" s="10">
-        <v>60</v>
-      </c>
-      <c r="B61" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="E61" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="G61" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="H61" s="10">
-        <v>20</v>
-      </c>
-      <c r="I61" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="J61" s="10" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -3628,10 +3469,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B24F9BD-DBB3-4699-BEB1-125B6EBE7265}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3641,36 +3482,76 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>276</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>277</v>
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7BE5EF-E3DD-48AF-9CCD-DC8EADF57159}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>